<commit_message>
Excel Data and corresponding Feature file changed
</commit_message>
<xml_diff>
--- a/src/test/resources/excelData/PythonCodeExcel.xlsx
+++ b/src/test/resources/excelData/PythonCodeExcel.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>Code</t>
   </si>
@@ -71,21 +71,28 @@
   </si>
   <si>
     <t>No tests were collected</t>
+  </si>
+  <si>
+    <t>age = 20
+age_group = "Minor" if age &lt; 18 else "Adult"
+print(age_group)</t>
+  </si>
+  <si>
+    <t>Adult</t>
+  </si>
+  <si>
+    <t>x = "Minor" if age &lt; 5 else "Adult"
+print(x)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
@@ -94,7 +101,7 @@
       <name val="Arial"/>
     </font>
     <font>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
@@ -125,24 +132,23 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -361,8 +367,8 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="28.25"/>
-    <col customWidth="1" min="2" max="2" width="36.88"/>
+    <col customWidth="1" min="1" max="1" width="36.0"/>
+    <col customWidth="1" min="2" max="2" width="35.75"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -372,109 +378,101 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="4" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>